<commit_message>
8200 words, 47 pages.
</commit_message>
<xml_diff>
--- a/Documents/Window visualisation.xlsx
+++ b/Documents/Window visualisation.xlsx
@@ -740,8 +740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:ER55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DU14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="DR48" sqref="DR48"/>
+    <sheetView tabSelected="1" topLeftCell="CS1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="DS2" sqref="DS2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,6 +751,9 @@
     <col min="50" max="50" width="9.140625" style="10"/>
     <col min="61" max="61" width="9.140625" style="7"/>
     <col min="74" max="74" width="9.140625" style="10"/>
+    <col min="112" max="118" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="120" max="122" width="2.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:148" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>

</xml_diff>